<commit_message>
refined hts workflow for version 1
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_screening.xlsx
+++ b/config/default/forms/app/hts_screening.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="168">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -219,25 +219,22 @@
     <t xml:space="preserve">Encounter date can not be in the future</t>
   </si>
   <si>
+    <t xml:space="preserve">select_one service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hts_service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required service</t>
+  </si>
+  <si>
     <t xml:space="preserve">observation</t>
   </si>
   <si>
-    <t xml:space="preserve">select_one population_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_160112_populationType_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one department</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_159936_department_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Department</t>
+    <t xml:space="preserve">HTS eligibility screening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(${hts_service},’newOrRetest’)</t>
   </si>
   <si>
     <t xml:space="preserve">select_one yes_no</t>
@@ -294,13 +291,16 @@
     <t xml:space="preserve">screening_outcome_text</t>
   </si>
   <si>
-    <t xml:space="preserve">if(${_164401_everTestedByProvider_99DCT}='_1065_yes_99DCT' and ${duration_since_last_test} &gt; 12 and ${_159427_testResults_99DCT} != '_703_positive_99DCT', 'Eligible', if(${_164401_everTestedByProvider_99DCT}='_1066_no_99DCT', 'Eligible', 'Not eligible'))</t>
+    <t xml:space="preserve">if(${_164401_everTestedByProvider_99DCT}='_1065_yes_99DCT' and ${duration_since_last_test} &gt; 12 and ${_159427_testResults_99DCT} != '_703_positive_99DCT', 'Eligible', if(${_164401_everTestedByProvider_99DCT}='_1066_no_99DCT', 'Eligible', if(${_164401_everTestedByProvider_99DCT}='_1065_yes_99DCT' and ${_159427_testResults_99DCT} = '_703_positive_99DCT','Not eligible',if(${_164401_everTestedByProvider_99DCT}='_1065_yes_99DCT' and ${duration_since_last_test} &lt;= 12 and ${_159427_testResults_99DCT} = '_664_negative_99DCT', 'Not eligible',''))))</t>
   </si>
   <si>
     <t xml:space="preserve">outcome_header</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;span style='color:brown;'&gt;Screening outcome: ${screening_outcome_text} &lt;i class="fa fa-warning"&gt;&lt;/i&gt;&lt;/span&gt;</t>
+    <t xml:space="preserve">&lt;span style='color:brown;'&gt; &lt;i class="fa fa-warning"&gt; HTS screening status: ${screening_outcome_text}&lt;/i&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(${_164401_everTestedByProvider_99DCT},'_1065_yes_99DCT') or selected(${_164401_everTestedByProvider_99DCT},'_1066_no_99DCT')</t>
   </si>
   <si>
     <t xml:space="preserve">text</t>
@@ -351,156 +351,129 @@
     <t xml:space="preserve">Assessment findings&lt;I class="fa fa-user"&gt;&lt;/i&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">n_drinking_water_source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**_Population Type_**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hp</t>
+    <t xml:space="preserve">hiv_tested_before</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**_Tested for HIV before_**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(../../observation/_164401_everTestedByProvider_99DCT, '_1065_yes_99DCT')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">li</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(../../observation/_164401_everTestedByProvider_99DCT, '_1066_no_99DCT')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**_Test result_**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results_positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(../../observation/_159427_testResults_99DCT, '_703_positive_99DCT')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results_negative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(../../observation/_159427_testResults_99DCT, '_664_negative_99DCT')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testeligible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**_HTS eligibility_**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eligible_yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eligible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(../../observation/_162699_eligibleForTesting_99DCT, '_1065_yes_99DCT')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eligible_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not eligible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(../../observation/_162699_eligibleForTesting_99DCT, '_1066_no_99DCT')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audit_trail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">created_by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../../inputs/user/name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_1065_yes_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_1066_no_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">population_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_1065_HP_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">HP</t>
   </si>
   <si>
-    <t xml:space="preserve">selected(../../observation/_160112_populationType_99DCT, '_1065_HP_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">li</t>
-  </si>
-  <si>
-    <t xml:space="preserve">np</t>
+    <t xml:space="preserve">_1066_NP_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">NP</t>
   </si>
   <si>
-    <t xml:space="preserve">selected(../../observation/_160112_populationType_99DCT, '_1066_NP_99DCT')</t>
-  </si>
-  <si>
     <t xml:space="preserve">department</t>
   </si>
   <si>
-    <t xml:space="preserve">**_Department_**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">opd</t>
+    <t xml:space="preserve">_160542_OPD_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">OPD</t>
   </si>
   <si>
-    <t xml:space="preserve">selected(../../observation/_159936_department_99DCT, '_160542_OPD_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ipd</t>
+    <t xml:space="preserve">_5485_IPD_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">IPD</t>
   </si>
   <si>
-    <t xml:space="preserve">selected(../../observation/_159936_department_99DCT, '_5485_IPD_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hiv_tested_before</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**_Tested for HIV before_**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_164401_everTestedByProvider_99DCT, '_1065_yes_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_164401_everTestedByProvider_99DCT, '_1066_no_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**_Test result_**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results_positive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_159427_testResults_99DCT, '_703_positive_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results_negative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Negative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_159427_testResults_99DCT, '_664_negative_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testeligible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**_Client eligible for testing_**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eligible_yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_162699_eligibleForTesting_99DCT, '_1065_yes_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eligible_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_162699_eligibleForTesting_99DCT, '_1066_no_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audit_trail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">created_by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../../inputs/user/name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1065_yes_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1066_no_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">population_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1065_HP_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1066_NP_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_160542_OPD_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_5485_IPD_99DCT</t>
-  </si>
-  <si>
     <t xml:space="preserve">test_result</t>
   </si>
   <si>
@@ -510,6 +483,21 @@
     <t xml:space="preserve">_664_negative_99DCT</t>
   </si>
   <si>
+    <t xml:space="preserve">service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newOrRetest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New/Retest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmPositiveResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-test to confirm +ve results</t>
+  </si>
+  <si>
     <t xml:space="preserve">form_title</t>
   </si>
   <si>
@@ -528,7 +516,7 @@
     <t xml:space="preserve">instance_name</t>
   </si>
   <si>
-    <t xml:space="preserve">HTS Screening Form</t>
+    <t xml:space="preserve">HTS screening form</t>
   </si>
   <si>
     <t xml:space="preserve">hts_screening_form</t>
@@ -715,7 +703,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -754,10 +742,6 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2127,30 +2111,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL75"/>
+  <dimension ref="A1:AL65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="C49" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+      <selection pane="topRight" activeCell="C53" activeCellId="0" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.9081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.9948979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="59.5765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.484693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="113.841836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.6887755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="36.3571428571429"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="45.5357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="21.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.7959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.2551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="70.9132653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="92.515306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="135.801020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="45.5357142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="43.1989795918367"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="54.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="25.5561224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3288,21 +3272,21 @@
       <c r="X35" s="8"/>
       <c r="Y35" s="8"/>
     </row>
-    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="8"/>
+        <v>66</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
@@ -3325,24 +3309,27 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
+      <c r="C37" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
       <c r="O37" s="8"/>
@@ -3359,13 +3346,13 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>62</v>
@@ -3377,7 +3364,6 @@
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
       <c r="O38" s="8"/>
@@ -3392,26 +3378,29 @@
       <c r="X38" s="8"/>
       <c r="Y38" s="8"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E39" s="8"/>
+      <c r="E39" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
       <c r="O39" s="8"/>
@@ -3426,25 +3415,29 @@
       <c r="X39" s="8"/>
       <c r="Y39" s="8"/>
     </row>
-    <row r="40" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>62</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
+      <c r="G40" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
@@ -3463,30 +3456,26 @@
       <c r="X40" s="8"/>
       <c r="Y40" s="8"/>
     </row>
-    <row r="41" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>62</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D41" s="8"/>
       <c r="E41" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F41" s="8"/>
-      <c r="G41" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
@@ -3505,25 +3494,23 @@
       <c r="Y41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="s">
-        <v>46</v>
+      <c r="A42" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
-      <c r="I42" s="8" t="s">
-        <v>83</v>
-      </c>
+      <c r="I42" s="8"/>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
@@ -3542,23 +3529,23 @@
       <c r="Y42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
-        <v>84</v>
+      <c r="A43" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="D43" s="8"/>
-      <c r="E43" s="8" t="s">
-        <v>78</v>
-      </c>
+      <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
+      <c r="I43" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
@@ -3576,12 +3563,12 @@
       <c r="X43" s="8"/>
       <c r="Y43" s="8"/>
     </row>
-    <row r="44" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="67" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>19</v>
@@ -3592,7 +3579,7 @@
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
@@ -3611,24 +3598,24 @@
       <c r="X44" s="8"/>
       <c r="Y44" s="8"/>
     </row>
-    <row r="45" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="54" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="E45" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
-      <c r="I45" s="8" t="s">
-        <v>90</v>
-      </c>
+      <c r="I45" s="8"/>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
@@ -3646,21 +3633,23 @@
       <c r="X45" s="8"/>
       <c r="Y45" s="8"/>
     </row>
-    <row r="46" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D46" s="8"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
@@ -3679,23 +3668,17 @@
       <c r="X46" s="8"/>
       <c r="Y46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>95</v>
-      </c>
+    <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
-      <c r="F47" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
@@ -3714,15 +3697,23 @@
       <c r="X47" s="8"/>
       <c r="Y47" s="8"/>
     </row>
-    <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="27.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
+        <v>13</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>98</v>
+      </c>
       <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
+      <c r="E48" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
@@ -3745,19 +3736,17 @@
     </row>
     <row r="49" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
-      <c r="F49" s="8" t="s">
-        <v>99</v>
-      </c>
+      <c r="F49" s="8"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
@@ -3780,17 +3769,19 @@
     </row>
     <row r="50" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>103</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
+      <c r="F50" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
@@ -3811,21 +3802,19 @@
       <c r="X50" s="8"/>
       <c r="Y50" s="8"/>
     </row>
-    <row r="51" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
-      <c r="F51" s="8" t="s">
-        <v>104</v>
-      </c>
+      <c r="F51" s="8"/>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
@@ -3846,19 +3835,21 @@
       <c r="X51" s="8"/>
       <c r="Y51" s="8"/>
     </row>
-    <row r="52" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
+      <c r="F52" s="8" t="s">
+        <v>96</v>
+      </c>
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
@@ -3879,21 +3870,19 @@
       <c r="X52" s="8"/>
       <c r="Y52" s="8"/>
     </row>
-    <row r="53" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="s">
-        <v>84</v>
+    <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
-      <c r="F53" s="8" t="s">
-        <v>96</v>
-      </c>
+      <c r="F53" s="8"/>
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
@@ -3914,19 +3903,23 @@
       <c r="X53" s="8"/>
       <c r="Y53" s="8"/>
     </row>
-    <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
-        <v>84</v>
+    <row r="54" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>110</v>
+        <v>62</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
+      <c r="E54" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -3948,21 +3941,21 @@
       <c r="Y54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>112</v>
+      <c r="A55" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
@@ -3984,56 +3977,56 @@
       <c r="X55" s="4"/>
       <c r="Y55" s="4"/>
     </row>
-    <row r="56" customFormat="false" ht="17.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4" t="s">
+    <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="F56" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
-      <c r="P56" s="4"/>
-      <c r="Q56" s="4"/>
-      <c r="R56" s="4"/>
-      <c r="S56" s="4"/>
-      <c r="T56" s="4"/>
-      <c r="U56" s="4"/>
-      <c r="V56" s="4"/>
-      <c r="W56" s="4"/>
-      <c r="X56" s="4"/>
-      <c r="Y56" s="4"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="8" t="s">
-        <v>84</v>
+      <c r="C56" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D56" s="8"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="8"/>
+      <c r="S56" s="8"/>
+      <c r="T56" s="8"/>
+      <c r="U56" s="8"/>
+      <c r="V56" s="8"/>
+      <c r="W56" s="8"/>
+      <c r="X56" s="8"/>
+      <c r="Y56" s="8"/>
+    </row>
+    <row r="57" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
+      <c r="E57" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
@@ -4056,127 +4049,127 @@
     </row>
     <row r="58" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D58" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D58" s="8"/>
       <c r="E58" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
-      <c r="Q58" s="4"/>
-      <c r="R58" s="4"/>
-      <c r="S58" s="4"/>
-      <c r="T58" s="4"/>
-      <c r="U58" s="4"/>
-      <c r="V58" s="4"/>
-      <c r="W58" s="4"/>
-      <c r="X58" s="4"/>
-      <c r="Y58" s="4"/>
-    </row>
-    <row r="59" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="8"/>
+      <c r="R58" s="8"/>
+      <c r="S58" s="8"/>
+      <c r="T58" s="8"/>
+      <c r="U58" s="8"/>
+      <c r="V58" s="8"/>
+      <c r="W58" s="8"/>
+      <c r="X58" s="8"/>
+      <c r="Y58" s="8"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="F59" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
-      <c r="Q59" s="4"/>
-      <c r="R59" s="4"/>
-      <c r="S59" s="4"/>
-      <c r="T59" s="4"/>
-      <c r="U59" s="4"/>
-      <c r="V59" s="4"/>
-      <c r="W59" s="4"/>
-      <c r="X59" s="4"/>
-      <c r="Y59" s="4"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B60" s="8" t="s">
+      <c r="C59" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="8"/>
+      <c r="N59" s="8"/>
+      <c r="O59" s="8"/>
+      <c r="P59" s="8"/>
+      <c r="Q59" s="8"/>
+      <c r="R59" s="8"/>
+      <c r="S59" s="8"/>
+      <c r="T59" s="8"/>
+      <c r="U59" s="8"/>
+      <c r="V59" s="8"/>
+      <c r="W59" s="8"/>
+      <c r="X59" s="8"/>
+      <c r="Y59" s="8"/>
+    </row>
+    <row r="60" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="8"/>
-      <c r="L60" s="8"/>
-      <c r="M60" s="8"/>
-      <c r="N60" s="8"/>
-      <c r="O60" s="8"/>
-      <c r="P60" s="8"/>
-      <c r="Q60" s="8"/>
-      <c r="R60" s="8"/>
-      <c r="S60" s="8"/>
-      <c r="T60" s="8"/>
-      <c r="U60" s="8"/>
-      <c r="V60" s="8"/>
-      <c r="W60" s="8"/>
-      <c r="X60" s="8"/>
-      <c r="Y60" s="8"/>
+      <c r="C60" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+      <c r="W60" s="4"/>
+      <c r="X60" s="4"/>
+      <c r="Y60" s="4"/>
     </row>
     <row r="61" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>128</v>
+      <c r="A61" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
@@ -4198,56 +4191,40 @@
       <c r="X61" s="4"/>
       <c r="Y61" s="4"/>
     </row>
-    <row r="62" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
-      <c r="N62" s="4"/>
-      <c r="O62" s="4"/>
-      <c r="P62" s="4"/>
-      <c r="Q62" s="4"/>
-      <c r="R62" s="4"/>
-      <c r="S62" s="4"/>
-      <c r="T62" s="4"/>
-      <c r="U62" s="4"/>
-      <c r="V62" s="4"/>
-      <c r="W62" s="4"/>
-      <c r="X62" s="4"/>
-      <c r="Y62" s="4"/>
+    <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="8"/>
+      <c r="M62" s="8"/>
+      <c r="N62" s="8"/>
+      <c r="O62" s="8"/>
+      <c r="P62" s="8"/>
+      <c r="Q62" s="8"/>
+      <c r="R62" s="8"/>
+      <c r="S62" s="8"/>
+      <c r="T62" s="8"/>
+      <c r="U62" s="8"/>
+      <c r="V62" s="8"/>
+      <c r="W62" s="8"/>
+      <c r="X62" s="8"/>
+      <c r="Y62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>134</v>
-      </c>
+      <c r="A63" s="4"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
       <c r="D63" s="8"/>
       <c r="E63" s="4"/>
-      <c r="F63" s="8"/>
+      <c r="F63" s="4"/>
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
       <c r="I63" s="8"/>
@@ -4268,23 +4245,13 @@
       <c r="X63" s="8"/>
       <c r="Y63" s="8"/>
     </row>
-    <row r="64" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>136</v>
-      </c>
+    <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="4"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
       <c r="D64" s="8"/>
-      <c r="E64" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
@@ -4305,23 +4272,15 @@
       <c r="X64" s="8"/>
       <c r="Y64" s="8"/>
     </row>
-    <row r="65" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>139</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
       <c r="D65" s="8"/>
-      <c r="E65" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
       <c r="I65" s="8"/>
@@ -4342,289 +4301,82 @@
       <c r="X65" s="8"/>
       <c r="Y65" s="8"/>
     </row>
-    <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="8"/>
-      <c r="K66" s="8"/>
-      <c r="L66" s="8"/>
-      <c r="M66" s="8"/>
-      <c r="N66" s="8"/>
-      <c r="O66" s="8"/>
-      <c r="P66" s="8"/>
-      <c r="Q66" s="8"/>
-      <c r="R66" s="8"/>
-      <c r="S66" s="8"/>
-      <c r="T66" s="8"/>
-      <c r="U66" s="8"/>
-      <c r="V66" s="8"/>
-      <c r="W66" s="8"/>
-      <c r="X66" s="8"/>
-      <c r="Y66" s="8"/>
-    </row>
-    <row r="67" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-      <c r="P67" s="4"/>
-      <c r="Q67" s="4"/>
-      <c r="R67" s="4"/>
-      <c r="S67" s="4"/>
-      <c r="T67" s="4"/>
-      <c r="U67" s="4"/>
-      <c r="V67" s="4"/>
-      <c r="W67" s="4"/>
-      <c r="X67" s="4"/>
-      <c r="Y67" s="4"/>
-    </row>
-    <row r="68" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
-      <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-      <c r="P68" s="4"/>
-      <c r="Q68" s="4"/>
-      <c r="R68" s="4"/>
-      <c r="S68" s="4"/>
-      <c r="T68" s="4"/>
-      <c r="U68" s="4"/>
-      <c r="V68" s="4"/>
-      <c r="W68" s="4"/>
-      <c r="X68" s="4"/>
-      <c r="Y68" s="4"/>
-    </row>
-    <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="8"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
-      <c r="I69" s="8"/>
-      <c r="J69" s="8"/>
-      <c r="K69" s="8"/>
-      <c r="L69" s="8"/>
-      <c r="M69" s="8"/>
-      <c r="N69" s="8"/>
-      <c r="O69" s="8"/>
-      <c r="P69" s="8"/>
-      <c r="Q69" s="8"/>
-      <c r="R69" s="8"/>
-      <c r="S69" s="8"/>
-      <c r="T69" s="8"/>
-      <c r="U69" s="8"/>
-      <c r="V69" s="8"/>
-      <c r="W69" s="8"/>
-      <c r="X69" s="8"/>
-      <c r="Y69" s="8"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
-      <c r="L70" s="8"/>
-      <c r="M70" s="8"/>
-      <c r="N70" s="8"/>
-      <c r="O70" s="8"/>
-      <c r="P70" s="8"/>
-      <c r="Q70" s="8"/>
-      <c r="R70" s="8"/>
-      <c r="S70" s="8"/>
-      <c r="T70" s="8"/>
-      <c r="U70" s="8"/>
-      <c r="V70" s="8"/>
-      <c r="W70" s="8"/>
-      <c r="X70" s="8"/>
-      <c r="Y70" s="8"/>
-    </row>
-    <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
-      <c r="J71" s="8"/>
-      <c r="K71" s="8"/>
-      <c r="L71" s="8"/>
-      <c r="M71" s="8"/>
-      <c r="N71" s="8"/>
-      <c r="O71" s="8"/>
-      <c r="P71" s="8"/>
-      <c r="Q71" s="8"/>
-      <c r="R71" s="8"/>
-      <c r="S71" s="8"/>
-      <c r="T71" s="8"/>
-      <c r="U71" s="8"/>
-      <c r="V71" s="8"/>
-      <c r="W71" s="8"/>
-      <c r="X71" s="8"/>
-      <c r="Y71" s="8"/>
-    </row>
-    <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="4" t="s">
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="12"/>
+      <c r="M66" s="12"/>
+      <c r="N66" s="12"/>
+    </row>
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D67" s="14"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="15"/>
+    </row>
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="8"/>
-      <c r="H72" s="8"/>
-      <c r="I72" s="8"/>
-      <c r="J72" s="8"/>
-      <c r="K72" s="8"/>
-      <c r="L72" s="8"/>
-      <c r="M72" s="8"/>
-      <c r="N72" s="8"/>
-      <c r="O72" s="8"/>
-      <c r="P72" s="8"/>
-      <c r="Q72" s="8"/>
-      <c r="R72" s="8"/>
-      <c r="S72" s="8"/>
-      <c r="T72" s="8"/>
-      <c r="U72" s="8"/>
-      <c r="V72" s="8"/>
-      <c r="W72" s="8"/>
-      <c r="X72" s="8"/>
-      <c r="Y72" s="8"/>
-    </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G73" s="13"/>
-      <c r="H73" s="13"/>
-      <c r="I73" s="13"/>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
-      <c r="L73" s="13"/>
-      <c r="M73" s="13"/>
-      <c r="N73" s="13"/>
-    </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D74" s="15"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="16"/>
-      <c r="I74" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="J74" s="16"/>
-      <c r="K74" s="16"/>
-      <c r="L74" s="16"/>
-      <c r="M74" s="16"/>
-      <c r="N74" s="16"/>
-    </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="13"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
-      <c r="L75" s="13"/>
-      <c r="M75" s="13"/>
-      <c r="N75" s="13"/>
-    </row>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="12"/>
+      <c r="K68" s="12"/>
+      <c r="L68" s="12"/>
+      <c r="M68" s="12"/>
+      <c r="N68" s="12"/>
+    </row>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="B1">
     <cfRule type="cellIs" priority="2" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
@@ -4680,697 +4432,697 @@
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40:Y40">
+  <conditionalFormatting sqref="A39:Y39">
     <cfRule type="containsText" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40:Y40">
+  <conditionalFormatting sqref="A39:Y39">
     <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
+  <conditionalFormatting sqref="A39">
     <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
+  <conditionalFormatting sqref="A47">
     <cfRule type="containsText" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
+  <conditionalFormatting sqref="A47">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
-      <formula>AND($A48="begin group", NOT($B48 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
+      <formula>AND($A47="begin group", NOT($B47 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
-      <formula>AND($A48="end group", $B48 = "", $C48 = "", $D48 = "", $E48 = "", $F48 = "", $G48 = "", $H48 = "", $I48 = "", $J48 = "", $K48 = "", $L48 = "", $M48 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
+      <formula>AND($A47="end group", $B47 = "", $C47 = "", $D47 = "", $E47 = "", $F47 = "", $G47 = "", $H47 = "", $I47 = "", $J47 = "", $K47 = "", $L47 = "", $M47 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
     <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
+  <conditionalFormatting sqref="A47">
     <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
+  <conditionalFormatting sqref="A47">
     <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
-      <formula>AND($A48="begin repeat", NOT($B48 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
+      <formula>AND($A47="begin repeat", NOT($B47 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
     <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
-      <formula>AND($A48="end repeat", $B48 = "", $C48 = "", $D48 = "", $E48 = "", $F48 = "", $G48 = "", $H48 = "", $I48 = "", $J48 = "", $K48 = "", $L48 = "", $M48 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E38:E40">
+      <formula>AND($A47="end repeat", $B47 = "", $C47 = "", $D47 = "", $E47 = "", $F47 = "", $G47 = "", $H47 = "", $I47 = "", $J47 = "", $K47 = "", $L47 = "", $M47 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38:E39">
     <cfRule type="containsText" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E38:E40">
+  <conditionalFormatting sqref="E38:E39">
     <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:A40">
+  <conditionalFormatting sqref="A38:A39">
     <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39:E40">
+  <conditionalFormatting sqref="E38:E39">
     <cfRule type="containsText" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
+  <conditionalFormatting sqref="E38">
     <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
-      <formula>AND($A39="end group", $B39 = "", $C39 = "", $D39 = "", $E39 = "", $F39 = "", $G39 = "", $H39 = "", $I39 = "", $J39 = "", $K39 = "", $I39 = "", $M39 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E39:E40">
+      <formula>AND($A38="end group", $B38 = "", $C38 = "", $D38 = "", $E38 = "", $F38 = "", $G38 = "", $H38 = "", $I38 = "", $J38 = "", $K38 = "", $I38 = "", $M38 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38:E39">
     <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
+  <conditionalFormatting sqref="E38">
     <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A39="end repeat", $B39 = "", $C39 = "", $D39 = "", $E39 = "", $F39 = "", $G39 = "", $H39 = "", $I39 = "", $J39 = "", $K39 = "", $I39 = "", $M39 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:Y35">
+      <formula>AND($A38="end repeat", $B38 = "", $C38 = "", $D38 = "", $E38 = "", $F38 = "", $G38 = "", $H38 = "", $I38 = "", $J38 = "", $K38 = "", $I38 = "", $M38 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35:Y36">
     <cfRule type="containsText" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="29"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A35:Y35">
+  <conditionalFormatting sqref="A35:Y36">
     <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
+  <conditionalFormatting sqref="A35:A36">
     <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:Y42">
+  <conditionalFormatting sqref="A40:Y41">
     <cfRule type="containsText" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:Y42">
+  <conditionalFormatting sqref="A40:Y41">
     <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
-      <formula>AND($A41="begin group", NOT($B41 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41:Y42">
+      <formula>AND($A40="begin group", NOT($B40 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:Y41">
     <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
-      <formula>AND($A41="end group", $B41 = "", $C41 = "", $D41 = "", $E41 = "", $F41 = "", $G41 = "", $H41 = "", $I41 = "", $J41 = "", $K41 = "", $L41 = "", $M41 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41:Y42">
+      <formula>AND($A40="end group", $B40 = "", $C40 = "", $D40 = "", $E40 = "", $F40 = "", $G40 = "", $H40 = "", $I40 = "", $J40 = "", $K40 = "", $L40 = "", $M40 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:Y41">
     <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:A42">
+  <conditionalFormatting sqref="A40:A41">
     <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:Y42">
+  <conditionalFormatting sqref="A40:Y41">
     <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
-      <formula>AND($A41="begin repeat", NOT($B41 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41:Y42">
+      <formula>AND($A40="begin repeat", NOT($B40 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:Y41">
     <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
-      <formula>AND($A41="end repeat", $B41 = "", $C41 = "", $D41 = "", $E41 = "", $F41 = "", $G41 = "", $H41 = "", $I41 = "", $J41 = "", $K41 = "", $L41 = "", $M41 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I41:I42">
+      <formula>AND($A40="end repeat", $B40 = "", $C40 = "", $D40 = "", $E40 = "", $F40 = "", $G40 = "", $H40 = "", $I40 = "", $J40 = "", $K40 = "", $L40 = "", $M40 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40:I41">
     <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>AND($I41 = "", $A41 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C41:C42">
+      <formula>AND($I40 = "", $A40 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40:C41">
     <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
-      <formula>AND(AND(NOT($A41 = "end group"), NOT($A41 = "end repeat"), NOT($A41 = "")), $C41 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B41:B42">
+      <formula>AND(AND(NOT($A40 = "end group"), NOT($A40 = "end repeat"), NOT($A40 = "")), $C40 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40:B41">
     <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
-      <formula>AND(AND(NOT($A41 = "end group"), NOT($A41 = "end repeat"), NOT($A41 = "")), $B41 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H41:H42">
+      <formula>AND(AND(NOT($A40 = "end group"), NOT($A40 = "end repeat"), NOT($A40 = "")), $B40 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H40:H41">
     <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
-      <formula>AND(NOT($G41 = ""), $H41 = "")</formula>
+      <formula>AND(NOT($G40 = ""), $H40 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
     <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
-      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1021, "begin group") = COUNTIF($A$1:$A$1021, "end group"))</formula>
+      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1014, "begin group") = COUNTIF($A$1:$A$1014, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
     <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
-      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1012, "begin group") = COUNTIF($A$1:$A$1021, "end group")))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47:Y47">
+      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1005, "begin group") = COUNTIF($A$1:$A$1014, "end group")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:Y46">
     <cfRule type="containsText" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="45"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A47:Y47">
+  <conditionalFormatting sqref="A46:Y46">
     <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
-      <formula>AND($A47="begin group", NOT($B47 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47:Y47">
+      <formula>AND($A46="begin group", NOT($B46 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:Y46">
     <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
-      <formula>AND($A47="end group", $B47 = "", $C47 = "", $D47 = "", $E47 = "", $F47 = "", $G47 = "", $H47 = "", $I47 = "", $J47 = "", $K47 = "", $L47 = "", $M47 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47:Y47">
+      <formula>AND($A46="end group", $B46 = "", $C46 = "", $D46 = "", $E46 = "", $F46 = "", $G46 = "", $H46 = "", $I46 = "", $J46 = "", $K46 = "", $L46 = "", $M46 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:Y46">
     <cfRule type="cellIs" priority="50" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
+  <conditionalFormatting sqref="I46">
     <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
-      <formula>AND($I47 = "", $A47 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
+      <formula>AND($I46 = "", $A46 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
     <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>AND(AND(NOT($A47 = "end group"), NOT($A47 = "end repeat"), NOT($A47 = "")), $C47 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
+      <formula>AND(AND(NOT($A46 = "end group"), NOT($A46 = "end repeat"), NOT($A46 = "")), $C46 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46">
     <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
-      <formula>AND(AND(NOT($A47 = "end group"), NOT($A47 = "end repeat"), NOT($A47 = "")), $B47 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
+      <formula>AND(AND(NOT($A46 = "end group"), NOT($A46 = "end repeat"), NOT($A46 = "")), $B46 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
     <cfRule type="cellIs" priority="54" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
+  <conditionalFormatting sqref="B46">
     <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
-      <formula>COUNTIF($B$2:$B$1050,B47)&gt;1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
+      <formula>COUNTIF($B$2:$B$1043,B46)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H46">
     <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
-      <formula>AND(NOT($G47 = ""), $H47 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47:Y47">
+      <formula>AND(NOT($G46 = ""), $H46 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:Y46">
     <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
-      <formula>AND($A47="begin repeat", NOT($B47 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47:Y47">
+      <formula>AND($A46="begin repeat", NOT($B46 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:Y46">
     <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
-      <formula>AND($A47="end repeat", $B47 = "", $C47 = "", $D47 = "", $E47 = "", $F47 = "", $G47 = "", $H47 = "", $I47 = "", $J47 = "", $K47 = "", $L47 = "", $M47 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E61:E63">
+      <formula>AND($A46="end repeat", $B46 = "", $C46 = "", $D46 = "", $E46 = "", $F46 = "", $G46 = "", $H46 = "", $I46 = "", $J46 = "", $K46 = "", $L46 = "", $M46 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54:E56">
     <cfRule type="containsText" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="57"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E61:E63">
+  <conditionalFormatting sqref="E54:E56">
     <cfRule type="cellIs" priority="60" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E61:E63">
+  <conditionalFormatting sqref="E54:E56">
     <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
-      <formula>AND($A61="begin group", NOT($B61 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E61:E63">
+      <formula>AND($A54="begin group", NOT($B54 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54:E56">
     <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
-      <formula>AND($A61="end group", $B61 = "", $C61 = "", $D61 = "", $E61 = "", $F61 = "", $G61 = "", $H61 = "", $I61 = "", $J61 = "", $K61 = "", $L61 = "", $M61 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E61:E63">
+      <formula>AND($A54="end group", $B54 = "", $C54 = "", $D54 = "", $E54 = "", $F54 = "", $G54 = "", $H54 = "", $I54 = "", $J54 = "", $K54 = "", $L54 = "", $M54 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54:E56">
     <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
-      <formula>AND($A61="begin repeat", NOT($B61 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E61:E63">
+      <formula>AND($A54="begin repeat", NOT($B54 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54:E56">
     <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
-      <formula>AND($A61="end repeat", $B61 = "", $C61 = "", $D61 = "", $E61 = "", $F61 = "", $G61 = "", $H61 = "", $I61 = "", $J61 = "", $K61 = "", $L61 = "", $M61 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63">
+      <formula>AND($A54="end repeat", $B54 = "", $C54 = "", $D54 = "", $E54 = "", $F54 = "", $G54 = "", $H54 = "", $I54 = "", $J54 = "", $K54 = "", $L54 = "", $M54 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
     <cfRule type="cellIs" priority="65" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A65:Y65">
+  <conditionalFormatting sqref="A58:Y58">
     <cfRule type="containsText" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A65:Y65">
+  <conditionalFormatting sqref="A58:Y58">
     <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
-      <formula>AND($A65="begin group", NOT($B65 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65:Y65">
+      <formula>AND($A58="begin group", NOT($B58 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58:Y58">
     <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
-      <formula>AND($A65="end group", $B65 = "", $C65 = "", $D65 = "", $E65 = "", $F65 = "", $G65 = "", $H65 = "", $I65 = "", $J65 = "", $K65 = "", $L65 = "", $M65 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65:Y65">
+      <formula>AND($A58="end group", $B58 = "", $C58 = "", $D58 = "", $E58 = "", $F58 = "", $G58 = "", $H58 = "", $I58 = "", $J58 = "", $K58 = "", $L58 = "", $M58 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58:Y58">
     <cfRule type="cellIs" priority="69" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
+  <conditionalFormatting sqref="I58">
     <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
-      <formula>AND($I65 = "", $A65 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
+      <formula>AND($I58 = "", $A58 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
-      <formula>AND(AND(NOT($A65 = "end group"), NOT($A65 = "end repeat"), NOT($A65 = "")), $C65 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B65">
+      <formula>AND(AND(NOT($A58 = "end group"), NOT($A58 = "end repeat"), NOT($A58 = "")), $C58 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
     <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
-      <formula>AND(AND(NOT($A65 = "end group"), NOT($A65 = "end repeat"), NOT($A65 = "")), $B65 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
+      <formula>AND(AND(NOT($A58 = "end group"), NOT($A58 = "end repeat"), NOT($A58 = "")), $B58 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
     <cfRule type="cellIs" priority="73" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H65">
+  <conditionalFormatting sqref="H58">
     <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
-      <formula>AND(NOT($G65 = ""), $H65 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65:Y65">
+      <formula>AND(NOT($G58 = ""), $H58 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58:Y58">
     <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
-      <formula>AND($A65="begin repeat", NOT($B65 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65:Y65">
+      <formula>AND($A58="begin repeat", NOT($B58 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58:Y58">
     <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
-      <formula>AND($A65="end repeat", $B65 = "", $C65 = "", $D65 = "", $E65 = "", $F65 = "", $G65 = "", $H65 = "", $I65 = "", $J65 = "", $K65 = "", $L65 = "", $M65 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:Y70">
+      <formula>AND($A58="end repeat", $B58 = "", $C58 = "", $D58 = "", $E58 = "", $F58 = "", $G58 = "", $H58 = "", $I58 = "", $J58 = "", $K58 = "", $L58 = "", $M58 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:Y63">
     <cfRule type="containsText" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="75"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A70:Y70">
+  <conditionalFormatting sqref="A63:Y63">
     <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
-      <formula>AND($A70="begin group", NOT($B70 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:Y70">
+      <formula>AND($A63="begin group", NOT($B63 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:Y63">
     <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
-      <formula>AND($A70="end group", $B70 = "", $C70 = "", $D70 = "", $E70 = "", $F70 = "", $G70 = "", $H70 = "", $I70 = "", $J70 = "", $K70 = "", $L70 = "", $M70 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:Y70">
+      <formula>AND($A63="end group", $B63 = "", $C63 = "", $D63 = "", $E63 = "", $F63 = "", $G63 = "", $H63 = "", $I63 = "", $J63 = "", $K63 = "", $L63 = "", $M63 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:Y63">
     <cfRule type="cellIs" priority="80" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I70">
+  <conditionalFormatting sqref="I63">
     <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
-      <formula>AND($I70 = "", $A70 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C70">
+      <formula>AND($I63 = "", $A63 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
     <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
-      <formula>AND(AND(NOT($A70 = "end group"), NOT($A70 = "end repeat"), NOT($A70 = "")), $C70 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
+      <formula>AND(AND(NOT($A63 = "end group"), NOT($A63 = "end repeat"), NOT($A63 = "")), $C63 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B63">
     <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
-      <formula>AND(AND(NOT($A70 = "end group"), NOT($A70 = "end repeat"), NOT($A70 = "")), $B70 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70">
+      <formula>AND(AND(NOT($A63 = "end group"), NOT($A63 = "end repeat"), NOT($A63 = "")), $B63 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63">
     <cfRule type="cellIs" priority="84" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H70">
+  <conditionalFormatting sqref="H63">
     <cfRule type="expression" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
-      <formula>AND(NOT($G70 = ""), $H70 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:Y70">
+      <formula>AND(NOT($G63 = ""), $H63 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:Y63">
     <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
-      <formula>AND($A70="begin repeat", NOT($B70 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:Y70">
+      <formula>AND($A63="begin repeat", NOT($B63 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:Y63">
     <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
-      <formula>AND($A70="end repeat", $B70 = "", $C70 = "", $D70 = "", $E70 = "", $F70 = "", $G70 = "", $H70 = "", $I70 = "", $J70 = "", $K70 = "", $L70 = "", $M70 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71:Y71">
+      <formula>AND($A63="end repeat", $B63 = "", $C63 = "", $D63 = "", $E63 = "", $F63 = "", $G63 = "", $H63 = "", $I63 = "", $J63 = "", $K63 = "", $L63 = "", $M63 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64:Y64">
     <cfRule type="containsText" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="86"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A71:Y71">
+  <conditionalFormatting sqref="A64:Y64">
     <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
-      <formula>AND($A71="begin group", NOT($B71 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71:Y71">
+      <formula>AND($A64="begin group", NOT($B64 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64:Y64">
     <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
-      <formula>AND($A71="end group", $B71 = "", $C71 = "", $D71 = "", $E71 = "", $F71 = "", $G71 = "", $H71 = "", $I71 = "", $J71 = "", $K71 = "", $L71 = "", $M71 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71:Y71">
+      <formula>AND($A64="end group", $B64 = "", $C64 = "", $D64 = "", $E64 = "", $F64 = "", $G64 = "", $H64 = "", $I64 = "", $J64 = "", $K64 = "", $L64 = "", $M64 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64:Y64">
     <cfRule type="cellIs" priority="91" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I71">
+  <conditionalFormatting sqref="I64">
     <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
-      <formula>AND($I71 = "", $A71 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C71">
+      <formula>AND($I64 = "", $A64 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
     <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
-      <formula>AND(AND(NOT($A71 = "end group"), NOT($A71 = "end repeat"), NOT($A71 = "")), $C71 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71">
+      <formula>AND(AND(NOT($A64 = "end group"), NOT($A64 = "end repeat"), NOT($A64 = "")), $C64 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B64">
     <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
-      <formula>AND(AND(NOT($A71 = "end group"), NOT($A71 = "end repeat"), NOT($A71 = "")), $B71 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71">
+      <formula>AND(AND(NOT($A64 = "end group"), NOT($A64 = "end repeat"), NOT($A64 = "")), $B64 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64">
     <cfRule type="cellIs" priority="95" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H71">
+  <conditionalFormatting sqref="H64">
     <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
-      <formula>AND(NOT($G71 = ""), $H71 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71:Y71">
+      <formula>AND(NOT($G64 = ""), $H64 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64:Y64">
     <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95">
-      <formula>AND($A71="begin repeat", NOT($B71 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71:Y71">
+      <formula>AND($A64="begin repeat", NOT($B64 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64:Y64">
     <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
-      <formula>AND($A71="end repeat", $B71 = "", $C71 = "", $D71 = "", $E71 = "", $F71 = "", $G71 = "", $H71 = "", $I71 = "", $J71 = "", $K71 = "", $L71 = "", $M71 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
+      <formula>AND($A64="end repeat", $B64 = "", $C64 = "", $D64 = "", $E64 = "", $F64 = "", $G64 = "", $H64 = "", $I64 = "", $J64 = "", $K64 = "", $L64 = "", $M64 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
     <cfRule type="containsText" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="97"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
+  <conditionalFormatting sqref="A65">
     <cfRule type="expression" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98">
-      <formula>AND($A72="begin group", NOT($B72 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
+      <formula>AND($A65="begin group", NOT($B65 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
     <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
-      <formula>AND($A72="end group", $B72 = "", $C72 = "", $D72 = "", $E72 = "", $F72 = "", $G72 = "", $H72 = "", $I72 = "", $J72 = "", $K72 = "", $L72 = "", $M72 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
+      <formula>AND($A65="end group", $B65 = "", $C65 = "", $D65 = "", $E65 = "", $F65 = "", $G65 = "", $H65 = "", $I65 = "", $J65 = "", $K65 = "", $L65 = "", $M65 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
     <cfRule type="cellIs" priority="102" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
+  <conditionalFormatting sqref="A65">
     <cfRule type="cellIs" priority="103" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
+  <conditionalFormatting sqref="A65">
     <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
-      <formula>AND($A72="begin repeat", NOT($B72 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
+      <formula>AND($A65="begin repeat", NOT($B65 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
     <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103">
-      <formula>AND($A72="end repeat", $B72 = "", $C72 = "", $D72 = "", $E72 = "", $F72 = "", $G72 = "", $H72 = "", $I72 = "", $J72 = "", $K72 = "", $L72 = "", $M72 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+      <formula>AND($A65="end repeat", $B65 = "", $C65 = "", $D65 = "", $E65 = "", $F65 = "", $G65 = "", $H65 = "", $I65 = "", $J65 = "", $K65 = "", $L65 = "", $M65 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
     <cfRule type="containsText" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="104"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+  <conditionalFormatting sqref="E62">
     <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105">
-      <formula>AND($A69="begin group", NOT($B69 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+      <formula>AND($A62="begin group", NOT($B62 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
     <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106">
-      <formula>AND($A69="end group", $B69 = "", $C69 = "", $D69 = "", $E69 = "", $F69 = "", $G69 = "", $H69 = "", $I69 = "", $J69 = "", $K69 = "", $L69 = "", $M69 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+      <formula>AND($A62="end group", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
     <cfRule type="cellIs" priority="109" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+  <conditionalFormatting sqref="E62">
     <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108">
-      <formula>AND($A69="begin repeat", NOT($B69 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+      <formula>AND($A62="begin repeat", NOT($B62 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
     <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109">
-      <formula>AND($A69="end repeat", $B69 = "", $C69 = "", $D69 = "", $E69 = "", $F69 = "", $G69 = "", $H69 = "", $I69 = "", $J69 = "", $K69 = "", $L69 = "", $M69 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+      <formula>AND($A62="end repeat", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
     <cfRule type="containsText" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="110"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+  <conditionalFormatting sqref="E62">
     <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111">
-      <formula>AND($A69="begin group", NOT($B69 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+      <formula>AND($A62="begin group", NOT($B62 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
     <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112">
-      <formula>AND($A69="end group", $B69 = "", $C69 = "", $D69 = "", $E69 = "", $F69 = "", $G69 = "", $H69 = "", $I69 = "", $J69 = "", $K69 = "", $L69 = "", $M69 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+      <formula>AND($A62="end group", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
     <cfRule type="cellIs" priority="115" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+  <conditionalFormatting sqref="E62">
     <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114">
-      <formula>AND($A69="begin repeat", NOT($B69 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+      <formula>AND($A62="begin repeat", NOT($B62 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
     <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115">
-      <formula>AND($A69="end repeat", $B69 = "", $C69 = "", $D69 = "", $E69 = "", $F69 = "", $G69 = "", $H69 = "", $I69 = "", $J69 = "", $K69 = "", $L69 = "", $M69 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I69">
+      <formula>AND($A62="end repeat", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I62">
     <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116">
-      <formula>AND($I69 = "", $A69 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C69">
+      <formula>AND($I62 = "", $A62 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
     <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117">
-      <formula>AND(AND(NOT($A69 = "end group"), NOT($A69 = "end repeat"), NOT($A69 = "")), $C69 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B69">
+      <formula>AND(AND(NOT($A62 = "end group"), NOT($A62 = "end repeat"), NOT($A62 = "")), $C62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62">
     <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118">
-      <formula>AND(AND(NOT($A69 = "end group"), NOT($A69 = "end repeat"), NOT($A69 = "")), $B69 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
+      <formula>AND(AND(NOT($A62 = "end group"), NOT($A62 = "end repeat"), NOT($A62 = "")), $B62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62">
     <cfRule type="cellIs" priority="121" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H69">
+  <conditionalFormatting sqref="H62">
     <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120">
-      <formula>AND(NOT($G69 = ""), $H69 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71">
+      <formula>AND(NOT($G62 = ""), $H62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B64">
     <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121">
-      <formula>COUNTIF($B$2:$B$1042,B71)&gt;1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44:Y44">
+      <formula>COUNTIF($B$2:$B$1035,B64)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y43">
     <cfRule type="containsText" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A44:Y44">
+  <conditionalFormatting sqref="A43:Y43">
     <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
-      <formula>AND($A44="begin group", NOT($B44 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44:Y44">
+      <formula>AND($A43="begin group", NOT($B43 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y43">
     <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
-      <formula>AND($A44="end group", $B44 = "", $C44 = "", $D44 = "", $E44 = "", $F44 = "", $G44 = "", $H44 = "", $I44 = "", $J44 = "", $K44 = "", $L44 = "", $M44 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44:Y44">
+      <formula>AND($A43="end group", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $G43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y43">
     <cfRule type="cellIs" priority="127" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
+  <conditionalFormatting sqref="A43">
     <cfRule type="cellIs" priority="128" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y43">
+    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
+      <formula>AND($A43="begin repeat", NOT($B43 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y43">
+    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
+      <formula>AND($A43="end repeat", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $G43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43">
+    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>AND($I43 = "", $A43 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
+    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+      <formula>AND(AND(NOT($A43 = "end group"), NOT($A43 = "end repeat"), NOT($A43 = "")), $C43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43">
+    <cfRule type="expression" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+      <formula>AND(AND(NOT($A43 = "end group"), NOT($A43 = "end repeat"), NOT($A43 = "")), $B43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43">
+    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+      <formula>AND(NOT($G43 = ""), $H43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A44:Y44">
-    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
-      <formula>AND($A44="begin repeat", NOT($B44 = ""))</formula>
-    </cfRule>
+    <cfRule type="containsText" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44:Y44">
-    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
-      <formula>AND($A44="end repeat", $B44 = "", $C44 = "", $D44 = "", $E44 = "", $F44 = "", $G44 = "", $H44 = "", $I44 = "", $J44 = "", $K44 = "", $L44 = "", $M44 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
-    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>AND($I44 = "", $A44 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
-      <formula>AND(AND(NOT($A44 = "end group"), NOT($A44 = "end repeat"), NOT($A44 = "")), $C44 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
-    <cfRule type="expression" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
-      <formula>AND(AND(NOT($A44 = "end group"), NOT($A44 = "end repeat"), NOT($A44 = "")), $B44 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H44">
-    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
-      <formula>AND(NOT($G44 = ""), $H44 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Y45">
-    <cfRule type="containsText" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="32"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Y45">
     <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
-      <formula>AND($A45="begin group", NOT($B45 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Y45">
+      <formula>AND($A44="begin group", NOT($B44 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44:Y44">
     <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
-      <formula>AND($A45="end group", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Y45">
+      <formula>AND($A44="end group", $B44 = "", $C44 = "", $D44 = "", $E44 = "", $F44 = "", $G44 = "", $H44 = "", $I44 = "", $J44 = "", $K44 = "", $L44 = "", $M44 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44:Y44">
     <cfRule type="cellIs" priority="138" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
+  <conditionalFormatting sqref="A44">
     <cfRule type="cellIs" priority="139" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Y45">
+  <conditionalFormatting sqref="A44:Y44">
     <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
-      <formula>AND($A45="begin repeat", NOT($B45 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Y45">
+      <formula>AND($A44="begin repeat", NOT($B44 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44:Y44">
     <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
-      <formula>AND($A45="end repeat", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
+      <formula>AND($A44="end repeat", $B44 = "", $C44 = "", $D44 = "", $E44 = "", $F44 = "", $G44 = "", $H44 = "", $I44 = "", $J44 = "", $K44 = "", $L44 = "", $M44 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>AND($I44 = "", $A44 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
+    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+      <formula>AND(AND(NOT($A44 = "end group"), NOT($A44 = "end repeat"), NOT($A44 = "")), $C44 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44">
+    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+      <formula>AND(AND(NOT($A44 = "end group"), NOT($A44 = "end repeat"), NOT($A44 = "")), $B44 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H44">
+    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+      <formula>AND(NOT($G44 = ""), $H44 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45">
-    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
       <formula>AND($I45 = "", $A45 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
       <formula>AND(AND(NOT($A45 = "end group"), NOT($A45 = "end repeat"), NOT($A45 = "")), $C45 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
       <formula>AND(AND(NOT($A45 = "end group"), NOT($A45 = "end repeat"), NOT($A45 = "")), $B45 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H45">
-    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
-      <formula>AND(NOT($G45 = ""), $H45 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
-    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
-      <formula>AND($I46 = "", $A46 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
-      <formula>AND(AND(NOT($A46 = "end group"), NOT($A46 = "end repeat"), NOT($A46 = "")), $C46 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46">
-    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
-      <formula>AND(AND(NOT($A46 = "end group"), NOT($A46 = "end repeat"), NOT($A46 = "")), $B46 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
+  <conditionalFormatting sqref="A45">
     <cfRule type="cellIs" priority="149" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H46">
+  <conditionalFormatting sqref="H45">
     <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
-      <formula>AND(NOT($G46 = ""), $H46 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
+      <formula>AND(NOT($G45 = ""), $H45 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
     <cfRule type="containsText" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="122"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
+  <conditionalFormatting sqref="E45">
     <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123">
-      <formula>AND($A46="begin group", NOT($B46 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
+      <formula>AND($A45="begin group", NOT($B45 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
     <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124">
-      <formula>AND($A46="end group", $B46 = "", $C46 = "", $D46 = "", $E46 = "", $F46 = "", $G46 = "", $H46 = "", $I46 = "", $J46 = "", $K46 = "", $L46 = "", $M46 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
+      <formula>AND($A45="end group", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
     <cfRule type="cellIs" priority="154" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
+  <conditionalFormatting sqref="E45">
     <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126">
-      <formula>AND($A46="begin repeat", NOT($B46 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
+      <formula>AND($A45="begin repeat", NOT($B45 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
     <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127">
-      <formula>AND($A46="end repeat", $B46 = "", $C46 = "", $D46 = "", $E46 = "", $F46 = "", $G46 = "", $H46 = "", $I46 = "", $J46 = "", $K46 = "", $L46 = "", $M46 = "")</formula>
+      <formula>AND($A45="end repeat", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2 D8:D12 D14:D45 D47:D72" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2 D8:D12 D14:D44 D46:D65" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3:D7 D73:D75" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3:D7 D66:D68" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D46" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D45" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5395,190 +5147,212 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.515306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.4744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="21.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.9948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="25.5561224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C14" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="C15" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="B18" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C18" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" s="11" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="C19" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
     </row>
     <row r="1048504" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048505" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5610,49 +5384,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.6887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="21.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="25.5561224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="18" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="B2" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="C2" s="19" t="n">
+        <f aca="true">NOW()</f>
+        <v>44084.703221705</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="E2" s="10" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="20" t="n">
-        <f aca="true">NOW()</f>
-        <v>44070.4654421184</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="F2" s="11"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
validate nok relationship based on age. add linkage to hts services. validate prep appointment verification date against encounter date
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_screening.xlsx
+++ b/config/default/forms/app/hts_screening.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="170">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -496,6 +496,12 @@
   </si>
   <si>
     <t xml:space="preserve">Re-test to confirm +ve results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linkage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linkage</t>
   </si>
   <si>
     <t xml:space="preserve">form_title</t>
@@ -2116,25 +2122,25 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="C49" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
-      <selection pane="topRight" activeCell="C53" activeCellId="0" sqref="C53"/>
+      <selection pane="topRight" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="70.9132653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="92.515306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="135.801020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="45.5357142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="43.1989795918367"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="54.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.7755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.3469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.5051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9897959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="73.4336734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="95.8418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="140.75"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="47.1581632653061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="44.7295918367347"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="56.3367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="26.4591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5147,15 +5153,15 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.7091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.6071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.9948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="26.4591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5352,6 +5358,17 @@
       </c>
       <c r="C19" s="0" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="1048504" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5384,47 +5401,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="26.4591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C2" s="19" t="n">
         <f aca="true">NOW()</f>
-        <v>44084.703221705</v>
+        <v>44105.5141512753</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F2" s="10"/>
     </row>

</xml_diff>

<commit_message>
fix mapping of variables for referral and linkage facilities. Fix workflow in hts screening form
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_screening.xlsx
+++ b/config/default/forms/app/hts_screening.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="186">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -264,19 +264,34 @@
     <t xml:space="preserve">Do you remember date when you were last tested?</t>
   </si>
   <si>
-    <t xml:space="preserve">selected(${_164401_everTestedByProvider_99DCT},'_1065_yes_99DCT') </t>
+    <t xml:space="preserve">selected(${_159427_testResults_99DCT},'_664_negative_99DCT')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exact_test_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date tested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(${_164401_everTestedByProvider_99DCT},'_1065_yes_99DCT') and selected(${patient_Test_Date_Known},'_1065_yes_99DCT')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date tested can not be in the future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estimated_test_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated date tested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(${_164401_everTestedByProvider_99DCT},'_1065_yes_99DCT') and selected(${patient_Test_Date_Known},'_1066_no_99DCT')</t>
   </si>
   <si>
     <t xml:space="preserve">_164400_dateTested_99DCT</t>
   </si>
   <si>
-    <t xml:space="preserve">Date tested</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(${_164401_everTestedByProvider_99DCT},'_1065_yes_99DCT') and selected(${patient_Test_Date_Known},'_1065_yes_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date tested can not be in the future</t>
+    <t xml:space="preserve">if(${exact_test_date}!=’’,${exact_test_date},${estimated_test_date})</t>
   </si>
   <si>
     <t xml:space="preserve">duration_since_last_test</t>
@@ -285,57 +300,21 @@
     <t xml:space="preserve">difference-in-months( ${_164400_dateTested_99DCT} , today() )</t>
   </si>
   <si>
-    <t xml:space="preserve">integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patient_ageYears</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Months since last tested:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(${patient_Test_Date_Known},'_1066_no_99DCT') </t>
-  </si>
-  <si>
-    <t xml:space="preserve">. &gt;= 0 and . &lt;= 110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age must be between 0 and 110</t>
+    <t xml:space="preserve">_162699_eligibleForTesting_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if(${_164401_everTestedByProvider_99DCT}='_1065_yes_99DCT' and ${duration_since_last_test} &gt; 12 and ${_159427_testResults_99DCT} != '_703_positive_99DCT', '_1065_yes_99DCT', if(${_164401_everTestedByProvider_99DCT}='_1066_no_99DCT', '_1065_yes_99DCT', '_1066_no_99DCT'))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">screening_outcome_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if(${_164401_everTestedByProvider_99DCT}='_1065_yes_99DCT' and ${duration_since_last_test} &gt; 12 and ${_159427_testResults_99DCT} != '_703_positive_99DCT', 'Eligible', if(${_164401_everTestedByProvider_99DCT}='_1066_no_99DCT', 'Eligible', if(${_164401_everTestedByProvider_99DCT}='_1065_yes_99DCT' and ${_159427_testResults_99DCT} = '_703_positive_99DCT','Not eligible',if(${_164401_everTestedByProvider_99DCT}='_1065_yes_99DCT' and ${duration_since_last_test} &lt;= 12 and ${_159427_testResults_99DCT} = '_664_negative_99DCT', 'Not eligible',''))))</t>
   </si>
   <si>
     <t xml:space="preserve">note</t>
   </si>
   <si>
-    <t xml:space="preserve">no_of_days_note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Months since last tested: ${duration_since_last_test}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(${_164401_everTestedByProvider_99DCT},'_1065_yes_99DCT') and selected(${patient_Test_Date_Known},'_1066_no_99DCT') </t>
-  </si>
-  <si>
-    <t xml:space="preserve">. &gt;= 1 and . &lt;= 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_162699_eligibleForTesting_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if(${_164401_everTestedByProvider_99DCT}='_1065_yes_99DCT' and ${duration_since_last_test} &gt; 12 and ${_159427_testResults_99DCT} != '_703_positive_99DCT', '_1065_yes_99DCT', if(${_164401_everTestedByProvider_99DCT}='_1066_no_99DCT', '_1065_yes_99DCT', '_1066_no_99DCT'))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">screening_outcome_text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if(${_164401_everTestedByProvider_99DCT}='_1065_yes_99DCT' and ${duration_since_last_test} &gt; 12 and ${_159427_testResults_99DCT} != '_703_positive_99DCT', 'Eligible', if(${_164401_everTestedByProvider_99DCT}='_1066_no_99DCT', 'Eligible', if(${_164401_everTestedByProvider_99DCT}='_1065_yes_99DCT' and ${_159427_testResults_99DCT} = '_703_positive_99DCT','Not eligible',if(${_164401_everTestedByProvider_99DCT}='_1065_yes_99DCT' and ${duration_since_last_test} &lt;= 12 and ${_159427_testResults_99DCT} = '_664_negative_99DCT', 'Not eligible',''))))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${screening_outcome_text}</t>
-  </si>
-  <si>
     <t xml:space="preserve">outcome</t>
   </si>
   <si>
@@ -351,7 +330,13 @@
     <t xml:space="preserve">&lt;span style="color:red"&gt;HTS screening status: Not eligible&lt;/span&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">${screening_outcome_text}='Not eligible'</t>
+    <t xml:space="preserve">${screening_outcome_text}='Not eligible' and ${_164400_dateTested_99DCT} !=’’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ever_tested_positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(${_164401_everTestedByProvider_99DCT},'_1065_yes_99DCT') and selected(${_159427_testResults_99DCT},'_703_positive_99DCT')</t>
   </si>
   <si>
     <t xml:space="preserve">text</t>
@@ -722,7 +707,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -866,421 +851,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="95">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
+  <dxfs count="49">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -1733,7 +1304,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF980000"/>
+      <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -1743,12 +1314,12 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFF2CC"/>
-      <rgbColor rgb="FFCFE2F3"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFC27BA0"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFD9D2E9"/>
+      <rgbColor rgb="FFCFE2F3"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1758,13 +1329,13 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFD9EAD3"/>
-      <rgbColor rgb="FFFCE5CD"/>
-      <rgbColor rgb="FFB7E1CD"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFEAD1DC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1794,27 +1365,27 @@
   <dimension ref="A1:AL65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2397959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="69.0255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6173469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="75.9540816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="99.265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="145.790816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.3571428571429"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="48.7755102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="46.3469387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="58.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="27.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.4642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="73.9744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="81.4438775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="106.551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="156.591836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.3367346938775"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="52.3775510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="49.6785714285714"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="62.6377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="29.3367346938775"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3121,7 +2692,7 @@
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
     </row>
-    <row r="41" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
         <v>59</v>
       </c>
@@ -3162,26 +2733,30 @@
       <c r="X41" s="8"/>
       <c r="Y41" s="8"/>
     </row>
-    <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>85</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="8"/>
+        <v>86</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="E42" s="8" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8" t="s">
-        <v>86</v>
-      </c>
+      <c r="G42" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I42" s="8"/>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
@@ -3199,56 +2774,63 @@
       <c r="X42" s="8"/>
       <c r="Y42" s="8"/>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" s="4" t="s">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="4" t="s">
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
+      <c r="V43" s="8"/>
+      <c r="W43" s="8"/>
+      <c r="X43" s="8"/>
+      <c r="Y43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-    </row>
-    <row r="44" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="C44" s="8" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="8" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="F44" s="8"/>
-      <c r="G44" s="8" t="s">
-        <v>97</v>
-      </c>
+      <c r="G44" s="8"/>
       <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
+      <c r="I44" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
@@ -3271,7 +2853,7 @@
         <v>46</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>19</v>
@@ -3282,7 +2864,7 @@
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
@@ -3306,7 +2888,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>19</v>
@@ -3317,7 +2899,7 @@
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
       <c r="I46" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
@@ -3336,18 +2918,20 @@
       <c r="X46" s="8"/>
       <c r="Y46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
+      <c r="E47" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
@@ -3369,19 +2953,19 @@
       <c r="X47" s="8"/>
       <c r="Y47" s="8"/>
     </row>
-    <row r="48" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
@@ -3404,19 +2988,19 @@
       <c r="X48" s="8"/>
       <c r="Y48" s="8"/>
     </row>
-    <row r="49" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
@@ -3441,18 +3025,18 @@
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
@@ -3508,17 +3092,17 @@
         <v>13</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
@@ -3542,13 +3126,13 @@
     </row>
     <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
@@ -3575,18 +3159,18 @@
     </row>
     <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
@@ -3610,13 +3194,13 @@
     </row>
     <row r="55" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
@@ -3643,18 +3227,18 @@
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
       <c r="F56" s="8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
@@ -3678,13 +3262,13 @@
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
@@ -3711,20 +3295,20 @@
     </row>
     <row r="58" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
@@ -3748,20 +3332,20 @@
     </row>
     <row r="59" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
@@ -3785,13 +3369,13 @@
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D60" s="8"/>
       <c r="E60" s="4"/>
@@ -3818,20 +3402,20 @@
     </row>
     <row r="61" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D61" s="8"/>
       <c r="E61" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
@@ -3855,20 +3439,20 @@
     </row>
     <row r="62" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D62" s="8"/>
       <c r="E62" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
@@ -3892,13 +3476,13 @@
     </row>
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
@@ -3925,20 +3509,20 @@
     </row>
     <row r="64" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
@@ -3962,20 +3546,20 @@
     </row>
     <row r="65" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
@@ -4112,7 +3696,7 @@
         <v>13</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>19</v>
@@ -4136,7 +3720,7 @@
         <v>46</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>19</v>
@@ -4147,7 +3731,7 @@
       <c r="G71" s="16"/>
       <c r="H71" s="16"/>
       <c r="I71" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="J71" s="16"/>
       <c r="K71" s="16"/>
@@ -4160,7 +3744,7 @@
         <v>46</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>19</v>
@@ -4171,7 +3755,7 @@
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
       <c r="I72" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
@@ -4216,785 +3800,944 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="notContainsText" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="label" dxfId="1"/>
+    <cfRule type="notContainsText" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="label" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" priority="4" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" priority="4" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"required"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" priority="5" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="5" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"relevant"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" priority="6" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="6" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"appearance"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="7" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" priority="7" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"constraint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="notContainsText" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="constraint_message" dxfId="4"/>
+    <cfRule type="notContainsText" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="constraint_message" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="cellIs" priority="9" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" priority="9" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"calculation"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" priority="10" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" priority="10" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"choice_filter"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="notContainsText" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="5"/>
+    <cfRule type="notContainsText" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" priority="12" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="12" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"default"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:Y1">
-    <cfRule type="cellIs" priority="13" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="cellIs" priority="13" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:Y39">
-    <cfRule type="containsText" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="6"/>
+    <cfRule type="containsText" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:Y39">
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39">
-    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="containsText" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+    <cfRule type="containsText" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A51="begin group", NOT($B51 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND($A51="end group", $B51 = "", $C51 = "", $D51 = "", $E51 = "", $F51 = "", $G51 = "", $H51 = "", $I51 = "", $J51 = "", $K51 = "", $L51 = "", $M51 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>AND($A51="begin repeat", NOT($B51 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>AND($A51="end repeat", $B51 = "", $C51 = "", $D51 = "", $E51 = "", $F51 = "", $G51 = "", $H51 = "", $I51 = "", $J51 = "", $K51 = "", $L51 = "", $M51 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38:E39">
-    <cfRule type="containsText" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="14"/>
+    <cfRule type="containsText" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38:E39">
-    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:A39">
-    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38:E39">
-    <cfRule type="containsText" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="17"/>
+    <cfRule type="containsText" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A38="end group", $B38 = "", $C38 = "", $D38 = "", $E38 = "", $F38 = "", $G38 = "", $H38 = "", $I38 = "", $J38 = "", $K38 = "", $I38 = "", $M38 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38:E39">
-    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A38="end repeat", $B38 = "", $C38 = "", $D38 = "", $E38 = "", $F38 = "", $G38 = "", $H38 = "", $I38 = "", $J38 = "", $K38 = "", $I38 = "", $M38 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:Y36">
-    <cfRule type="containsText" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="20"/>
+    <cfRule type="containsText" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:Y36">
-    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
+    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:A36">
-    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:Y42">
-    <cfRule type="containsText" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="22"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41:Y42">
-    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
+  <conditionalFormatting sqref="A43:Y44">
+    <cfRule type="containsText" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y44">
+    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A43="begin group", NOT($B43 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y44">
+    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A43="end group", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $G43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y44">
+    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:A44">
+    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y44">
+    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A43="begin repeat", NOT($B43 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y44">
+    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A43="end repeat", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $G43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43:I44">
+    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($I43 = "", $A43 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:C44">
+    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A43 = "end group"), NOT($A43 = "end repeat"), NOT($A43 = "")), $C43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43:B44">
+    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A43 = "end group"), NOT($A43 = "end repeat"), NOT($A43 = "")), $B43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43:H44">
+    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(NOT($G43 = ""), $H43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1019, "begin group") = COUNTIF($A$1:$A$1019, "end group"))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1010, "begin group") = COUNTIF($A$1:$A$1019, "end group")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:Y50">
+    <cfRule type="containsText" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:Y50">
+    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A50="begin group", NOT($B50 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:Y50">
+    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A50="end group", $B50 = "", $C50 = "", $D50 = "", $E50 = "", $F50 = "", $G50 = "", $H50 = "", $I50 = "", $J50 = "", $K50 = "", $L50 = "", $M50 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:Y50">
+    <cfRule type="cellIs" priority="50" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50">
+    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($I50 = "", $A50 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A50 = "end group"), NOT($A50 = "end repeat"), NOT($A50 = "")), $C50 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A50 = "end group"), NOT($A50 = "end repeat"), NOT($A50 = "")), $B50 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="cellIs" priority="54" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>COUNTIF($B$2:$B$1048,B50)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H50">
+    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(NOT($G50 = ""), $H50 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:Y50">
+    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A50="begin repeat", NOT($B50 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:Y50">
+    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A50="end repeat", $B50 = "", $C50 = "", $D50 = "", $E50 = "", $F50 = "", $G50 = "", $H50 = "", $I50 = "", $J50 = "", $K50 = "", $L50 = "", $M50 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58:E60">
+    <cfRule type="containsText" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58:E60">
+    <cfRule type="cellIs" priority="60" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58:E60">
+    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A58="begin group", NOT($B58 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58:E60">
+    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A58="end group", $B58 = "", $C58 = "", $D58 = "", $E58 = "", $F58 = "", $G58 = "", $H58 = "", $I58 = "", $J58 = "", $K58 = "", $L58 = "", $M58 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58:E60">
+    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A58="begin repeat", NOT($B58 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58:E60">
+    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A58="end repeat", $B58 = "", $C58 = "", $D58 = "", $E58 = "", $F58 = "", $G58 = "", $H58 = "", $I58 = "", $J58 = "", $K58 = "", $L58 = "", $M58 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="cellIs" priority="65" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:Y62">
+    <cfRule type="containsText" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:Y62">
+    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A62="begin group", NOT($B62 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:Y62">
+    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A62="end group", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:Y62">
+    <cfRule type="cellIs" priority="69" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I62">
+    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($I62 = "", $A62 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A62 = "end group"), NOT($A62 = "end repeat"), NOT($A62 = "")), $C62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62">
+    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A62 = "end group"), NOT($A62 = "end repeat"), NOT($A62 = "")), $B62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62">
+    <cfRule type="cellIs" priority="73" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62">
+    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(NOT($G62 = ""), $H62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:Y62">
+    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A62="begin repeat", NOT($B62 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:Y62">
+    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A62="end repeat", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67:Y67">
+    <cfRule type="containsText" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67:Y67">
+    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A67="begin group", NOT($B67 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67:Y67">
+    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A67="end group", $B67 = "", $C67 = "", $D67 = "", $E67 = "", $F67 = "", $G67 = "", $H67 = "", $I67 = "", $J67 = "", $K67 = "", $L67 = "", $M67 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67:Y67">
+    <cfRule type="cellIs" priority="80" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I67">
+    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($I67 = "", $A67 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
+    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A67 = "end group"), NOT($A67 = "end repeat"), NOT($A67 = "")), $C67 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B67">
+    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A67 = "end group"), NOT($A67 = "end repeat"), NOT($A67 = "")), $B67 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="cellIs" priority="84" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H67">
+    <cfRule type="expression" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(NOT($G67 = ""), $H67 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67:Y67">
+    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A67="begin repeat", NOT($B67 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67:Y67">
+    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A67="end repeat", $B67 = "", $C67 = "", $D67 = "", $E67 = "", $F67 = "", $G67 = "", $H67 = "", $I67 = "", $J67 = "", $K67 = "", $L67 = "", $M67 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:Y68">
+    <cfRule type="containsText" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:Y68">
+    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A68="begin group", NOT($B68 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:Y68">
+    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A68="end group", $B68 = "", $C68 = "", $D68 = "", $E68 = "", $F68 = "", $G68 = "", $H68 = "", $I68 = "", $J68 = "", $K68 = "", $L68 = "", $M68 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:Y68">
+    <cfRule type="cellIs" priority="91" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I68">
+    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($I68 = "", $A68 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68">
+    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A68 = "end group"), NOT($A68 = "end repeat"), NOT($A68 = "")), $C68 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B68">
+    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A68 = "end group"), NOT($A68 = "end repeat"), NOT($A68 = "")), $B68 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="cellIs" priority="95" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H68">
+    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(NOT($G68 = ""), $H68 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:Y68">
+    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+      <formula>AND($A68="begin repeat", NOT($B68 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:Y68">
+    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+      <formula>AND($A68="end repeat", $B68 = "", $C68 = "", $D68 = "", $E68 = "", $F68 = "", $G68 = "", $H68 = "", $I68 = "", $J68 = "", $K68 = "", $L68 = "", $M68 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="containsText" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="expression" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+      <formula>AND($A69="begin group", NOT($B69 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+      <formula>AND($A69="end group", $B69 = "", $C69 = "", $D69 = "", $E69 = "", $F69 = "", $G69 = "", $H69 = "", $I69 = "", $J69 = "", $K69 = "", $L69 = "", $M69 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="cellIs" priority="102" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="cellIs" priority="103" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+      <formula>AND($A69="begin repeat", NOT($B69 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+      <formula>AND($A69="end repeat", $B69 = "", $C69 = "", $D69 = "", $E69 = "", $F69 = "", $G69 = "", $H69 = "", $I69 = "", $J69 = "", $K69 = "", $L69 = "", $M69 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="containsText" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+      <formula>AND($A66="begin group", NOT($B66 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+      <formula>AND($A66="end group", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="cellIs" priority="109" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+      <formula>AND($A66="begin repeat", NOT($B66 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+      <formula>AND($A66="end repeat", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="containsText" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+      <formula>AND($A66="begin group", NOT($B66 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+      <formula>AND($A66="end group", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="cellIs" priority="115" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+      <formula>AND($A66="begin repeat", NOT($B66 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+      <formula>AND($A66="end repeat", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I66">
+    <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+      <formula>AND($I66 = "", $A66 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+      <formula>AND(AND(NOT($A66 = "end group"), NOT($A66 = "end repeat"), NOT($A66 = "")), $C66 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B66">
+    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+      <formula>AND(AND(NOT($A66 = "end group"), NOT($A66 = "end repeat"), NOT($A66 = "")), $B66 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="cellIs" priority="121" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66">
+    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
+      <formula>AND(NOT($G66 = ""), $H66 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B68">
+    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
+      <formula>COUNTIF($B$2:$B$1040,B68)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:Y45">
+    <cfRule type="containsText" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:Y45">
+    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
+      <formula>AND($A45="begin group", NOT($B45 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:Y45">
+    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+      <formula>AND($A45="end group", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:Y45">
+    <cfRule type="cellIs" priority="127" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
+    <cfRule type="cellIs" priority="128" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:Y45">
+    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
+      <formula>AND($A45="begin repeat", NOT($B45 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:Y45">
+    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
+      <formula>AND($A45="end repeat", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I45">
+    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
+      <formula>AND($I45 = "", $A45 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45">
+    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
+      <formula>AND(AND(NOT($A45 = "end group"), NOT($A45 = "end repeat"), NOT($A45 = "")), $C45 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="expression" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
+      <formula>AND(AND(NOT($A45 = "end group"), NOT($A45 = "end repeat"), NOT($A45 = "")), $B45 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45">
+    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
+      <formula>AND(NOT($G45 = ""), $H45 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:Y46">
+    <cfRule type="containsText" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:Y46">
+    <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>AND($A46="begin group", NOT($B46 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:Y46">
+    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>AND($A46="end group", $B46 = "", $C46 = "", $D46 = "", $E46 = "", $F46 = "", $G46 = "", $H46 = "", $I46 = "", $J46 = "", $K46 = "", $L46 = "", $M46 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:Y46">
+    <cfRule type="cellIs" priority="138" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46">
+    <cfRule type="cellIs" priority="139" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:Y46">
+    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>AND($A46="begin repeat", NOT($B46 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:Y46">
+    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>AND($A46="end repeat", $B46 = "", $C46 = "", $D46 = "", $E46 = "", $F46 = "", $G46 = "", $H46 = "", $I46 = "", $J46 = "", $K46 = "", $L46 = "", $M46 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I46">
+    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>AND($I46 = "", $A46 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>AND(AND(NOT($A46 = "end group"), NOT($A46 = "end repeat"), NOT($A46 = "")), $C46 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46">
+    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>AND(AND(NOT($A46 = "end group"), NOT($A46 = "end repeat"), NOT($A46 = "")), $B46 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H46">
+    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>AND(NOT($G46 = ""), $H46 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I48">
+    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+      <formula>AND($I48 = "", $A48 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+      <formula>AND(AND(NOT($A48 = "end group"), NOT($A48 = "end repeat"), NOT($A48 = "")), $C48 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48">
+    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+      <formula>AND(AND(NOT($A48 = "end group"), NOT($A48 = "end repeat"), NOT($A48 = "")), $B48 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="cellIs" priority="149" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H48">
+    <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+      <formula>AND(NOT($G48 = ""), $H48 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="containsText" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="41"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+      <formula>AND($A48="begin group", NOT($B48 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+      <formula>AND($A48="end group", $B48 = "", $C48 = "", $D48 = "", $E48 = "", $F48 = "", $G48 = "", $H48 = "", $I48 = "", $J48 = "", $K48 = "", $L48 = "", $M48 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="cellIs" priority="154" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+      <formula>AND($A48="begin repeat", NOT($B48 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+      <formula>AND($A48="end repeat", $B48 = "", $C48 = "", $D48 = "", $E48 = "", $F48 = "", $G48 = "", $H48 = "", $I48 = "", $J48 = "", $K48 = "", $L48 = "", $M48 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I47">
+    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+      <formula>AND($I47 = "", $A47 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+      <formula>AND(AND(NOT($A47 = "end group"), NOT($A47 = "end repeat"), NOT($A47 = "")), $C47 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47">
+    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+      <formula>AND(AND(NOT($A47 = "end group"), NOT($A47 = "end repeat"), NOT($A47 = "")), $B47 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="cellIs" priority="160" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H47">
+    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+      <formula>AND(NOT($G47 = ""), $H47 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="containsText" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="43"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="expression" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
+      <formula>AND($A47="begin group", NOT($B47 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="expression" priority="164" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+      <formula>AND($A47="end group", $B47 = "", $C47 = "", $D47 = "", $E47 = "", $F47 = "", $G47 = "", $H47 = "", $I47 = "", $J47 = "", $K47 = "", $L47 = "", $M47 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="cellIs" priority="165" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="expression" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
+      <formula>AND($A47="begin repeat", NOT($B47 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
+      <formula>AND($A47="end repeat", $B47 = "", $C47 = "", $D47 = "", $E47 = "", $F47 = "", $G47 = "", $H47 = "", $I47 = "", $J47 = "", $K47 = "", $L47 = "", $M47 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:Y41">
+    <cfRule type="containsText" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:Y41">
+    <cfRule type="expression" priority="169" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A41="begin group", NOT($B41 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:Y42">
-    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+  <conditionalFormatting sqref="A41:Y41">
+    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A41="end group", $B41 = "", $C41 = "", $D41 = "", $E41 = "", $F41 = "", $G41 = "", $H41 = "", $I41 = "", $J41 = "", $K41 = "", $L41 = "", $M41 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:Y42">
-    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+  <conditionalFormatting sqref="A41:Y41">
+    <cfRule type="cellIs" priority="171" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:A42">
-    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+  <conditionalFormatting sqref="A41">
+    <cfRule type="cellIs" priority="172" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:Y42">
-    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+  <conditionalFormatting sqref="A41:Y41">
+    <cfRule type="expression" priority="173" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A41="begin repeat", NOT($B41 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:Y42">
-    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+  <conditionalFormatting sqref="A41:Y41">
+    <cfRule type="expression" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A41="end repeat", $B41 = "", $C41 = "", $D41 = "", $E41 = "", $F41 = "", $G41 = "", $H41 = "", $I41 = "", $J41 = "", $K41 = "", $L41 = "", $M41 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I41:I42">
-    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+  <conditionalFormatting sqref="I41">
+    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($I41 = "", $A41 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41:C42">
-    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+  <conditionalFormatting sqref="C41">
+    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND(AND(NOT($A41 = "end group"), NOT($A41 = "end repeat"), NOT($A41 = "")), $C41 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B41:B42">
-    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+  <conditionalFormatting sqref="B41">
+    <cfRule type="expression" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND(AND(NOT($A41 = "end group"), NOT($A41 = "end repeat"), NOT($A41 = "")), $B41 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H41:H42">
-    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+  <conditionalFormatting sqref="H41">
+    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND(NOT($G41 = ""), $H41 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1019, "begin group") = COUNTIF($A$1:$A$1019, "end group"))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1010, "begin group") = COUNTIF($A$1:$A$1019, "end group")))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50:Y50">
-    <cfRule type="containsText" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50:Y50">
-    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A50="begin group", NOT($B50 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50:Y50">
-    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A50="end group", $B50 = "", $C50 = "", $D50 = "", $E50 = "", $F50 = "", $G50 = "", $H50 = "", $I50 = "", $J50 = "", $K50 = "", $L50 = "", $M50 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50:Y50">
-    <cfRule type="cellIs" priority="50" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+  <conditionalFormatting sqref="A42:Y42">
+    <cfRule type="containsText" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42:Y42">
+    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A42="begin group", NOT($B42 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42:Y42">
+    <cfRule type="expression" priority="181" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A42="end group", $B42 = "", $C42 = "", $D42 = "", $E42 = "", $F42 = "", $G42 = "", $H42 = "", $I42 = "", $J42 = "", $K42 = "", $L42 = "", $M42 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42:Y42">
+    <cfRule type="cellIs" priority="182" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I50">
-    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($I50 = "", $A50 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(AND(NOT($A50 = "end group"), NOT($A50 = "end repeat"), NOT($A50 = "")), $C50 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B50">
-    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(AND(NOT($A50 = "end group"), NOT($A50 = "end repeat"), NOT($A50 = "")), $B50 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50">
-    <cfRule type="cellIs" priority="54" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+  <conditionalFormatting sqref="A42">
+    <cfRule type="cellIs" priority="183" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50">
-    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>COUNTIF($B$2:$B$1048,B50)&gt;1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
-    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(NOT($G50 = ""), $H50 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50:Y50">
-    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A50="begin repeat", NOT($B50 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50:Y50">
-    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A50="end repeat", $B50 = "", $C50 = "", $D50 = "", $E50 = "", $F50 = "", $G50 = "", $H50 = "", $I50 = "", $J50 = "", $K50 = "", $L50 = "", $M50 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58:E60">
-    <cfRule type="containsText" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58:E60">
-    <cfRule type="cellIs" priority="60" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+  <conditionalFormatting sqref="A42:Y42">
+    <cfRule type="expression" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A42="begin repeat", NOT($B42 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42:Y42">
+    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A42="end repeat", $B42 = "", $C42 = "", $D42 = "", $E42 = "", $F42 = "", $G42 = "", $H42 = "", $I42 = "", $J42 = "", $K42 = "", $L42 = "", $M42 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I42">
+    <cfRule type="expression" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($I42 = "", $A42 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" priority="187" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A42 = "end group"), NOT($A42 = "end repeat"), NOT($A42 = "")), $C42 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
+    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A42 = "end group"), NOT($A42 = "end repeat"), NOT($A42 = "")), $B42 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H42">
+    <cfRule type="expression" priority="189" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(NOT($G42 = ""), $H42 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I49">
+    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+      <formula>AND($I48 = "", $A48 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49">
+    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+      <formula>AND(AND(NOT($A48 = "end group"), NOT($A48 = "end repeat"), NOT($A48 = "")), $C48 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49">
+    <cfRule type="expression" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+      <formula>AND(AND(NOT($A48 = "end group"), NOT($A48 = "end repeat"), NOT($A48 = "")), $B48 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="cellIs" priority="193" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H49">
+    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+      <formula>AND(NOT($G48 = ""), $H48 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49">
+    <cfRule type="containsText" priority="195" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="41"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49">
+    <cfRule type="expression" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+      <formula>AND($A48="begin group", NOT($B48 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49">
+    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+      <formula>AND($A48="end group", $B48 = "", $C48 = "", $D48 = "", $E48 = "", $F48 = "", $G48 = "", $H48 = "", $I48 = "", $J48 = "", $K48 = "", $L48 = "", $M48 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49">
+    <cfRule type="cellIs" priority="198" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E58:E60">
-    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A58="begin group", NOT($B58 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58:E60">
-    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A58="end group", $B58 = "", $C58 = "", $D58 = "", $E58 = "", $F58 = "", $G58 = "", $H58 = "", $I58 = "", $J58 = "", $K58 = "", $L58 = "", $M58 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58:E60">
-    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A58="begin repeat", NOT($B58 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58:E60">
-    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A58="end repeat", $B58 = "", $C58 = "", $D58 = "", $E58 = "", $F58 = "", $G58 = "", $H58 = "", $I58 = "", $J58 = "", $K58 = "", $L58 = "", $M58 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60">
-    <cfRule type="cellIs" priority="65" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:Y62">
-    <cfRule type="containsText" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:Y62">
-    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A62="begin group", NOT($B62 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:Y62">
-    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A62="end group", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:Y62">
-    <cfRule type="cellIs" priority="69" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I62">
-    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($I62 = "", $A62 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(AND(NOT($A62 = "end group"), NOT($A62 = "end repeat"), NOT($A62 = "")), $C62 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B62">
-    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(AND(NOT($A62 = "end group"), NOT($A62 = "end repeat"), NOT($A62 = "")), $B62 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62">
-    <cfRule type="cellIs" priority="73" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H62">
-    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(NOT($G62 = ""), $H62 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:Y62">
-    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A62="begin repeat", NOT($B62 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:Y62">
-    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A62="end repeat", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:Y67">
-    <cfRule type="containsText" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:Y67">
-    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A67="begin group", NOT($B67 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:Y67">
-    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A67="end group", $B67 = "", $C67 = "", $D67 = "", $E67 = "", $F67 = "", $G67 = "", $H67 = "", $I67 = "", $J67 = "", $K67 = "", $L67 = "", $M67 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:Y67">
-    <cfRule type="cellIs" priority="80" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I67">
-    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($I67 = "", $A67 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
-    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(AND(NOT($A67 = "end group"), NOT($A67 = "end repeat"), NOT($A67 = "")), $C67 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B67">
-    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(AND(NOT($A67 = "end group"), NOT($A67 = "end repeat"), NOT($A67 = "")), $B67 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="cellIs" priority="84" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H67">
-    <cfRule type="expression" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(NOT($G67 = ""), $H67 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:Y67">
-    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A67="begin repeat", NOT($B67 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:Y67">
-    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A67="end repeat", $B67 = "", $C67 = "", $D67 = "", $E67 = "", $F67 = "", $G67 = "", $H67 = "", $I67 = "", $J67 = "", $K67 = "", $L67 = "", $M67 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68:Y68">
-    <cfRule type="containsText" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68:Y68">
-    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A68="begin group", NOT($B68 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68:Y68">
-    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($A68="end group", $B68 = "", $C68 = "", $D68 = "", $E68 = "", $F68 = "", $G68 = "", $H68 = "", $I68 = "", $J68 = "", $K68 = "", $L68 = "", $M68 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68:Y68">
-    <cfRule type="cellIs" priority="91" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I68">
-    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND($I68 = "", $A68 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
-    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(AND(NOT($A68 = "end group"), NOT($A68 = "end repeat"), NOT($A68 = "")), $C68 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B68">
-    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
-      <formula>AND(AND(NOT($A68 = "end group"), NOT($A68 = "end repeat"), NOT($A68 = "")), $B68 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68">
-    <cfRule type="cellIs" priority="95" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H68">
-    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
-      <formula>AND(NOT($G68 = ""), $H68 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68:Y68">
-    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
-      <formula>AND($A68="begin repeat", NOT($B68 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68:Y68">
-    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
-      <formula>AND($A68="end repeat", $B68 = "", $C68 = "", $D68 = "", $E68 = "", $F68 = "", $G68 = "", $H68 = "", $I68 = "", $J68 = "", $K68 = "", $L68 = "", $M68 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="containsText" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="33"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="expression" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
-      <formula>AND($A69="begin group", NOT($B69 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
-      <formula>AND($A69="end group", $B69 = "", $C69 = "", $D69 = "", $E69 = "", $F69 = "", $G69 = "", $H69 = "", $I69 = "", $J69 = "", $K69 = "", $L69 = "", $M69 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="cellIs" priority="102" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="cellIs" priority="103" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
-      <formula>AND($A69="begin repeat", NOT($B69 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
-    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>AND($A69="end repeat", $B69 = "", $C69 = "", $D69 = "", $E69 = "", $F69 = "", $G69 = "", $H69 = "", $I69 = "", $J69 = "", $K69 = "", $L69 = "", $M69 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="containsText" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="40"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
-      <formula>AND($A66="begin group", NOT($B66 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
-      <formula>AND($A66="end group", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" priority="109" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
-      <formula>AND($A66="begin repeat", NOT($B66 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
-      <formula>AND($A66="end repeat", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="containsText" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="46"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
-      <formula>AND($A66="begin group", NOT($B66 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
-      <formula>AND($A66="end group", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" priority="115" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>AND($A66="begin repeat", NOT($B66 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
-      <formula>AND($A66="end repeat", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I66">
-    <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
-      <formula>AND($I66 = "", $A66 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
-    <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
-      <formula>AND(AND(NOT($A66 = "end group"), NOT($A66 = "end repeat"), NOT($A66 = "")), $C66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B66">
-    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
-      <formula>AND(AND(NOT($A66 = "end group"), NOT($A66 = "end repeat"), NOT($A66 = "")), $B66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
-    <cfRule type="cellIs" priority="121" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H66">
-    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
-      <formula>AND(NOT($G66 = ""), $H66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B68">
-    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
-      <formula>COUNTIF($B$2:$B$1040,B68)&gt;1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Y45">
-    <cfRule type="containsText" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="58"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Y45">
-    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
-      <formula>AND($A45="begin group", NOT($B45 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Y45">
-    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
-      <formula>AND($A45="end group", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Y45">
-    <cfRule type="cellIs" priority="127" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="cellIs" priority="128" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Y45">
-    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
-      <formula>AND($A45="begin repeat", NOT($B45 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Y45">
-    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
-      <formula>AND($A45="end repeat", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
-    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($I45 = "", $A45 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
-    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
-      <formula>AND(AND(NOT($A45 = "end group"), NOT($A45 = "end repeat"), NOT($A45 = "")), $C45 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
-    <cfRule type="expression" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
-      <formula>AND(AND(NOT($A45 = "end group"), NOT($A45 = "end repeat"), NOT($A45 = "")), $B45 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H45">
-    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
-      <formula>AND(NOT($G45 = ""), $H45 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46:Y47">
-    <cfRule type="containsText" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="68"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46:Y47">
-    <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
-      <formula>AND($A46="begin group", NOT($B46 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46:Y47">
-    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
-      <formula>AND($A46="end group", $B46 = "", $C46 = "", $D46 = "", $E46 = "", $F46 = "", $G46 = "", $H46 = "", $I46 = "", $J46 = "", $K46 = "", $L46 = "", $M46 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46:Y47">
-    <cfRule type="cellIs" priority="138" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46:A47">
-    <cfRule type="cellIs" priority="139" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46:Y47">
-    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
-      <formula>AND($A46="begin repeat", NOT($B46 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46:Y47">
-    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
-      <formula>AND($A46="end repeat", $B46 = "", $C46 = "", $D46 = "", $E46 = "", $F46 = "", $G46 = "", $H46 = "", $I46 = "", $J46 = "", $K46 = "", $L46 = "", $M46 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I46:I47">
-    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
-      <formula>AND($I46 = "", $A46 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46:C47">
-    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
-      <formula>AND(AND(NOT($A46 = "end group"), NOT($A46 = "end repeat"), NOT($A46 = "")), $C46 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46:B47">
-    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
-      <formula>AND(AND(NOT($A46 = "end group"), NOT($A46 = "end repeat"), NOT($A46 = "")), $B46 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H46:H47">
-    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
-      <formula>AND(NOT($G46 = ""), $H46 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I49">
-    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
-      <formula>AND($I49 = "", $A49 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
-      <formula>AND(AND(NOT($A49 = "end group"), NOT($A49 = "end repeat"), NOT($A49 = "")), $C49 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
-    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
-      <formula>AND(AND(NOT($A49 = "end group"), NOT($A49 = "end repeat"), NOT($A49 = "")), $B49 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="cellIs" priority="149" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H49">
-    <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
-      <formula>AND(NOT($G49 = ""), $H49 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="containsText" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="80"/>
+    <cfRule type="expression" priority="199" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+      <formula>AND($A48="begin repeat", NOT($B48 = ""))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
-      <formula>AND($A49="begin group", NOT($B49 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
-    <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
-      <formula>AND($A49="end group", $B49 = "", $C49 = "", $D49 = "", $E49 = "", $F49 = "", $G49 = "", $H49 = "", $I49 = "", $J49 = "", $K49 = "", $L49 = "", $M49 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
-    <cfRule type="cellIs" priority="154" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
-    <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
-      <formula>AND($A49="begin repeat", NOT($B49 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
-    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
-      <formula>AND($A49="end repeat", $B49 = "", $C49 = "", $D49 = "", $E49 = "", $F49 = "", $G49 = "", $H49 = "", $I49 = "", $J49 = "", $K49 = "", $L49 = "", $M49 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I48">
-    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
-      <formula>AND($I48 = "", $A48 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
-      <formula>AND(AND(NOT($A48 = "end group"), NOT($A48 = "end repeat"), NOT($A48 = "")), $C48 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B48">
-    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
-      <formula>AND(AND(NOT($A48 = "end group"), NOT($A48 = "end repeat"), NOT($A48 = "")), $B48 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
-    <cfRule type="cellIs" priority="160" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
-    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
-      <formula>AND(NOT($G48 = ""), $H48 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
-    <cfRule type="containsText" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="89"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
-    <cfRule type="expression" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
-      <formula>AND($A48="begin group", NOT($B48 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
-    <cfRule type="expression" priority="164" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
-      <formula>AND($A48="end group", $B48 = "", $C48 = "", $D48 = "", $E48 = "", $F48 = "", $G48 = "", $H48 = "", $I48 = "", $J48 = "", $K48 = "", $L48 = "", $M48 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
-    <cfRule type="cellIs" priority="165" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
-    <cfRule type="expression" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
-      <formula>AND($A48="begin repeat", NOT($B48 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
-    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
+    <cfRule type="expression" priority="200" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
       <formula>AND($A48="end repeat", $B48 = "", $C48 = "", $D48 = "", $E48 = "", $F48 = "", $G48 = "", $H48 = "", $I48 = "", $J48 = "", $K48 = "", $L48 = "", $M48 = "")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5024,20 +4767,20 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.1275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.7448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.3061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="27.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.1581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="82.8826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="29.3367346938775"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
@@ -5051,13 +4794,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
@@ -5065,13 +4808,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -5103,13 +4846,13 @@
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -5117,13 +4860,13 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -5139,13 +4882,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -5153,13 +4896,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
@@ -5183,13 +4926,13 @@
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
@@ -5197,13 +4940,13 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
@@ -5211,35 +4954,35 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>179</v>
-      </c>
       <c r="C20" s="0" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="1048504" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5272,47 +5015,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="27.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.7295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="27.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="29.3367346938775"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="29.3367346938775"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>181</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C2" s="20" t="n">
         <f aca="true">NOW()</f>
-        <v>44302.5981368549</v>
+        <v>44320.4059436666</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F2" s="11"/>
     </row>

</xml_diff>